<commit_message>
last corrections and new pdf v3
</commit_message>
<xml_diff>
--- a/VehicleTraceOldDataBackup.xlsx
+++ b/VehicleTraceOldDataBackup.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="26">
   <si>
     <t>Id</t>
   </si>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,6 +1195,41 @@
         <v>161580</v>
       </c>
     </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>13</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>2018</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21">
+        <v>220660</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>